<commit_message>
feat: Alteração da planilha dos professores
</commit_message>
<xml_diff>
--- a/src/main/resources/planilhas/DisponibilidadeProfessores.xlsx
+++ b/src/main/resources/planilhas/DisponibilidadeProfessores.xlsx
@@ -565,19 +565,19 @@
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -820,484 +820,924 @@
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="B2" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="B3" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G3" s="8"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="B4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G4" s="8"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="7"/>
+      <c r="B5" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G5" s="8"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
+      <c r="B6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1.0</v>
+      </c>
       <c r="G6" s="8"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="B7" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G7" s="8"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="B8" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="B9" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G9" s="8"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="B10" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G10" s="8"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="9"/>
+      <c r="B11" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1.0</v>
+      </c>
       <c r="G11" s="8"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="B12" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1.0</v>
+      </c>
       <c r="G12" s="8"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="7"/>
+      <c r="B13" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G13" s="8"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="9"/>
+      <c r="B14" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1.0</v>
+      </c>
       <c r="G14" s="8"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="B15" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G15" s="8"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="B16" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G16" s="8"/>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="7"/>
+      <c r="B17" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1.0</v>
+      </c>
       <c r="G17" s="8"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="7"/>
+      <c r="B18" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G18" s="8"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="B19" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G19" s="8"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="9"/>
+      <c r="B20" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F20" s="9">
+        <v>1.0</v>
+      </c>
       <c r="G20" s="8"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="B21" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G21" s="8"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="B22" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G22" s="8"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="B23" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G23" s="8"/>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="B24" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G24" s="8"/>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="B25" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G25" s="8"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="7"/>
+      <c r="B26" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G26" s="8"/>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="B27" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G27" s="8"/>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="B28" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G28" s="8"/>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="9"/>
+      <c r="B29" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F29" s="9">
+        <v>1.0</v>
+      </c>
       <c r="G29" s="8"/>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="B30" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E30" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G30" s="8"/>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="B31" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E31" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G31" s="8"/>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="B32" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F32" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G32" s="8"/>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="B33" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G33" s="8"/>
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="B34" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G34" s="8"/>
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="B35" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G35" s="8"/>
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="B36" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G36" s="8"/>
     </row>
     <row r="37">
       <c r="A37" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="B37" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G37" s="8"/>
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="9"/>
+      <c r="B38" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F38" s="9">
+        <v>1.0</v>
+      </c>
       <c r="G38" s="8"/>
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="7"/>
+      <c r="B39" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D39" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E39" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F39" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G39" s="8"/>
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="B40" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C40" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G40" s="8"/>
     </row>
     <row r="41">
       <c r="A41" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="7"/>
+      <c r="B41" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C41" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D41" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E41" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G41" s="8"/>
     </row>
     <row r="42">
       <c r="A42" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="B42" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C42" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D42" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G42" s="8"/>
     </row>
     <row r="43">
       <c r="A43" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="B43" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C43" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D43" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G43" s="8"/>
     </row>
     <row r="44">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="B44" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C44" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D44" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="F44" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G44" s="8"/>
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="7"/>
+      <c r="B45" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C45" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D45" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E45" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F45" s="7">
+        <v>0.0</v>
+      </c>
       <c r="G45" s="8"/>
     </row>
   </sheetData>

</xml_diff>